<commit_message>
t-test and formatting on spreadsheet
</commit_message>
<xml_diff>
--- a/report2/EnzymeLabData-1.xlsx
+++ b/report2/EnzymeLabData-1.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bio101\report2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1680" windowWidth="25485" windowHeight="14655" tabRatio="181"/>
+    <workbookView xWindow="3060" yWindow="1680" windowWidth="25485" windowHeight="14655" tabRatio="181" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>Food source</t>
   </si>
@@ -137,17 +133,68 @@
   <si>
     <t>BNAE Activity</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Equal Variances</t>
+  </si>
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Pooled Variance</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>ANAE T-test</t>
+  </si>
+  <si>
+    <t>BNAE T-test</t>
+  </si>
+  <si>
+    <t>Confidence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,16 +212,37 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -287,11 +355,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -323,9 +478,43 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -624,17 +813,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:3">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="25">
+        <v>0.17275404085692847</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.16034862587388751</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="25">
+        <v>4.4659462372220224E-2</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.10611329325749923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="25">
+        <v>33</v>
+      </c>
+      <c r="C6" s="25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="25">
+        <v>7.4898648998309877E-2</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="25">
+        <v>0</v>
+      </c>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="25">
+        <v>63</v>
+      </c>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="25">
+        <v>0.1827046436141801</v>
+      </c>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="25">
+        <v>0.42780822588369594</v>
+      </c>
+      <c r="C11" s="25"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="25">
+        <v>1.6694022221913696</v>
+      </c>
+      <c r="C12" s="25"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="25">
+        <v>0.85561645176739187</v>
+      </c>
+      <c r="C13" s="25"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="26">
+        <v>1.9983405224495088</v>
+      </c>
+      <c r="C14" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="10" topLeftCell="H40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="25" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
@@ -644,12 +972,13 @@
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.140625" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="17.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
     <col min="15" max="15" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -666,7 +995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -692,7 +1021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="B3" s="8"/>
       <c r="C3" s="8">
         <v>2</v>
@@ -715,7 +1044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="B4" s="8"/>
       <c r="C4" s="8">
         <v>3</v>
@@ -738,7 +1067,7 @@
         <v>0.16034862587388751</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="B5" s="8"/>
       <c r="C5" s="8">
         <v>4</v>
@@ -759,7 +1088,7 @@
         <v>0.32575035419397358</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="B6" s="8"/>
       <c r="C6" s="8">
         <v>5</v>
@@ -769,7 +1098,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="B7" s="8"/>
       <c r="C7" s="8">
         <v>6</v>
@@ -788,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="B8" s="8"/>
       <c r="C8" s="8">
         <v>7</v>
@@ -809,7 +1138,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="B9" s="8"/>
       <c r="C9" s="8">
         <v>8</v>
@@ -830,7 +1159,7 @@
         <v>4.9930767004645993E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="B10" s="8"/>
       <c r="C10" s="8">
         <v>9</v>
@@ -851,7 +1180,7 @@
         <v>0.1098898005251446</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="B11" s="8"/>
       <c r="C11" s="8">
         <v>10</v>
@@ -861,7 +1190,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1">
       <c r="B12" s="8"/>
       <c r="C12" s="8">
         <v>11</v>
@@ -870,8 +1199,14 @@
         <v>5.07077119821739E-2</v>
       </c>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="B13" s="8"/>
       <c r="C13" s="8">
         <v>12</v>
@@ -880,8 +1215,22 @@
         <v>7.6398745049243919E-2</v>
       </c>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="36"/>
+      <c r="I13" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="32"/>
+      <c r="M13" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
@@ -897,8 +1246,26 @@
       <c r="E14" s="1">
         <v>1.3100000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="29">
+        <v>0.17275404085692847</v>
+      </c>
+      <c r="J14" s="30">
+        <v>0.16034862587388751</v>
+      </c>
+      <c r="L14" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="25">
+        <v>0.10110664595549053</v>
+      </c>
+      <c r="N14" s="34">
+        <v>4.9930767004645993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15" s="8"/>
       <c r="C15" s="21" t="s">
         <v>17</v>
@@ -909,8 +1276,26 @@
       <c r="E15" s="2">
         <v>2.2000000000000001E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="29">
+        <v>4.4659462372220224E-2</v>
+      </c>
+      <c r="J15" s="30">
+        <v>0.10611329325749923</v>
+      </c>
+      <c r="L15" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="25">
+        <v>1.5056683576720797E-2</v>
+      </c>
+      <c r="N15" s="34">
+        <v>1.2075768259456072E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="B16" s="8"/>
       <c r="C16" s="21" t="s">
         <v>18</v>
@@ -919,8 +1304,26 @@
       <c r="E16" s="2">
         <v>2.9100000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H16" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="29">
+        <v>33</v>
+      </c>
+      <c r="J16" s="30">
+        <v>32</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="25">
+        <v>21</v>
+      </c>
+      <c r="N16" s="34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="B17" s="8"/>
       <c r="C17" s="21" t="s">
         <v>19</v>
@@ -929,8 +1332,24 @@
         <v>5.1691686177294215E-2</v>
       </c>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H17" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="29">
+        <v>63</v>
+      </c>
+      <c r="J17" s="30"/>
+      <c r="L17" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="25">
+        <v>43</v>
+      </c>
+      <c r="N17" s="34"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" s="8"/>
       <c r="C18" s="21" t="s">
         <v>20</v>
@@ -941,8 +1360,24 @@
       <c r="E18" s="15">
         <v>2.4490821175140766E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H18" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="40">
+        <v>0.1827046436141801</v>
+      </c>
+      <c r="J18" s="30"/>
+      <c r="L18" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="42">
+        <v>1.4760995551427978</v>
+      </c>
+      <c r="N18" s="34"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="B19" s="8"/>
       <c r="C19" s="21" t="s">
         <v>21</v>
@@ -953,8 +1388,24 @@
       <c r="E19" s="15">
         <v>1.5903518653502084E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H19" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="40">
+        <v>1.9983405224495088</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="L19" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" s="42">
+        <v>2.0166921734373453</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
         <v>13</v>
@@ -963,8 +1414,24 @@
         <v>3.9086062452399081E-2</v>
       </c>
       <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H20" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="40">
+        <v>0.85561645176739187</v>
+      </c>
+      <c r="J20" s="30"/>
+      <c r="L20" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="42">
+        <v>0.14720323947750413</v>
+      </c>
+      <c r="N20" s="34"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1">
       <c r="B21" s="8"/>
       <c r="C21" s="21" t="s">
         <v>15</v>
@@ -973,8 +1440,24 @@
         <v>8.6037735849056593E-2</v>
       </c>
       <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H21" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="48">
+        <f>ROUND((1-I20),4)</f>
+        <v>0.1444</v>
+      </c>
+      <c r="J21" s="31"/>
+      <c r="L21" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" s="49">
+        <f>ROUND((1-M20),4)</f>
+        <v>0.8528</v>
+      </c>
+      <c r="N21" s="35"/>
+    </row>
+    <row r="22" spans="1:17">
       <c r="B22" s="8"/>
       <c r="C22" s="22" t="s">
         <v>14</v>
@@ -984,7 +1467,7 @@
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1001,7 +1484,7 @@
         <v>0.19458874458874459</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8">
@@ -1014,7 +1497,7 @@
         <v>0.23342696629213483</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8">
@@ -1027,7 +1510,7 @@
         <v>8.6503067484662577E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8">
@@ -1040,7 +1523,7 @@
         <v>1.1335078534031413E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8">
@@ -1053,7 +1536,7 @@
         <v>1.7268518518518516E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8">
@@ -1066,7 +1549,7 @@
         <v>2.1363636363636362E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8">
@@ -1079,7 +1562,7 @@
         <v>1.3148148148148147E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8">
@@ -1092,7 +1575,7 @@
         <v>2.5677083333333333E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8">
@@ -1105,7 +1588,7 @@
         <v>3.7158469945355189E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8">
@@ -1118,7 +1601,7 @@
         <v>1.6787709497206704E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8">
@@ -1131,7 +1614,7 @@
         <v>3.6796874999999993E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8">
@@ -1144,7 +1627,7 @@
         <v>0.42245989304812831</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8">
@@ -1157,7 +1640,7 @@
         <v>0.33793103448275863</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
@@ -1174,7 +1657,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="B37" s="8"/>
       <c r="C37" s="8">
         <v>2</v>
@@ -1186,7 +1669,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="B38" s="8"/>
       <c r="C38" s="8">
         <v>3</v>
@@ -1198,7 +1681,7 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="B39" s="8"/>
       <c r="C39" s="8">
         <v>4</v>
@@ -1210,7 +1693,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="B40" s="8"/>
       <c r="C40" s="8">
         <v>5</v>
@@ -1223,7 +1706,7 @@
         <v>2.7407504835909617E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="B41" s="8"/>
       <c r="C41" s="8">
         <v>6</v>
@@ -1235,7 +1718,7 @@
         <v>2.454515892239989E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="B42" s="8"/>
       <c r="C42" s="8">
         <v>7</v>
@@ -1247,7 +1730,7 @@
         <v>1.4041797855630244E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="B43" s="8"/>
       <c r="C43" s="8">
         <v>8</v>
@@ -1259,7 +1742,7 @@
         <v>4.7755976162146422E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="B44" s="8"/>
       <c r="C44" s="8">
         <v>9</v>
@@ -1271,7 +1754,7 @@
         <v>6.0031208613782229E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="B45" s="8"/>
       <c r="C45" s="8">
         <v>10</v>
@@ -1281,7 +1764,7 @@
       </c>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="B46" s="8"/>
       <c r="C46" s="8">
         <v>11</v>
@@ -1291,7 +1774,7 @@
       </c>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="B47" s="9"/>
       <c r="C47" s="9">
         <v>12</v>
@@ -1301,7 +1784,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1799,7 @@
       </c>
       <c r="E48" s="10"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="C49" s="21" t="s">
@@ -1327,7 +1810,7 @@
       </c>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="C50" s="21" t="s">
@@ -1340,7 +1823,7 @@
         <v>8.2829791567655651E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="C51" s="21" t="s">
@@ -1351,7 +1834,7 @@
       </c>
       <c r="E51" s="11"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="C52" s="21" t="s">
@@ -1364,7 +1847,7 @@
         <v>1.1485317350853876E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="C53" s="21" t="s">
@@ -1375,7 +1858,7 @@
       </c>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="C54" s="21" t="s">
@@ -1386,7 +1869,7 @@
       </c>
       <c r="E54" s="15"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="C55" s="21" t="s">
@@ -1399,7 +1882,7 @@
         <v>1.0060603157113084E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="3"/>
       <c r="B56" s="9"/>
       <c r="C56" s="22" t="s">
@@ -1412,7 +1895,7 @@
         <v>9.2768748527839676E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>11</v>
       </c>
@@ -1429,7 +1912,7 @@
         <v>4.5769230769230763E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8">
@@ -1442,7 +1925,7 @@
         <v>7.3684210526315796E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8">
@@ -1455,7 +1938,7 @@
         <v>8.4210526315789472E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8">
@@ -1468,7 +1951,7 @@
         <v>2.9508196721311475E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8">
@@ -1481,7 +1964,7 @@
         <v>9.4904458598726107E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8">
@@ -1494,7 +1977,7 @@
         <v>2.8676470588235295E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8">
@@ -1507,7 +1990,7 @@
         <v>1.9201680672268909E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8">
@@ -1520,7 +2003,7 @@
         <v>3.6166666666666666E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8">
@@ -1533,7 +2016,7 @@
         <v>2.2628571428571428E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8">
@@ -1546,7 +2029,7 @@
         <v>1.2527472527472529E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="3"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9">
@@ -1571,13 +2054,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1588,13 +2071,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
"Make column graph in spreadsheet"
</commit_message>
<xml_diff>
--- a/report2/EnzymeLabData-1.xlsx
+++ b/report2/EnzymeLabData-1.xlsx
@@ -527,6 +527,396 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$H$5:$I$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.21132785517347263</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.32575035419397358</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$H$5:$I$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.21132785517347263</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.32575035419397358</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Mung Bean</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Cowpea</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.17275404085692847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16034862587388751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="47490560"/>
+        <c:axId val="47492096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="47490560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Food Source</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47492096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="47492096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>ANAE Activity (AU/</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" b="1">
+                    <a:latin typeface="Times New Roman"/>
+                    <a:cs typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:latin typeface="Times New Roman"/>
+                    <a:cs typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>g)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47490560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$H$10:$I$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.12270567866533642</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.1098898005251446</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$H$10:$I$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.12270567866533642</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.1098898005251446</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Mung Bean</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Cowpea</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.10110664595549053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9930767004645993E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50461696"/>
+        <c:axId val="51140864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50461696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Food Source</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51140864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51140864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0"/>
+                  <a:t>BNAE Activity (AU/</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1000" b="1" i="0" baseline="0"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0"/>
+                  <a:t>g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50461696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -953,13 +1343,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="25" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <pane xSplit="6" ySplit="22" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -969,16 +1359,16 @@
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -995,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1011,17 +1401,17 @@
       <c r="E2" s="2">
         <v>0.23899999999999999</v>
       </c>
+      <c r="G2" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="H2" s="7" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="B3" s="8"/>
       <c r="C3" s="8">
         <v>2</v>
@@ -1032,19 +1422,19 @@
       <c r="E3" s="2">
         <v>0.16700000000000001</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="7">
+      <c r="H3" s="7">
         <f>COUNT(D2:D35)</f>
         <v>33</v>
       </c>
-      <c r="J3" s="7">
+      <c r="I3" s="7">
         <f>COUNT(D36:D67)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="B4" s="8"/>
       <c r="C4" s="8">
         <v>3</v>
@@ -1055,19 +1445,19 @@
       <c r="E4" s="2">
         <v>0.17799999999999999</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="24">
+      <c r="H4" s="24">
         <f>AVERAGE(D2:D35)</f>
         <v>0.17275404085692847</v>
       </c>
-      <c r="J4" s="24">
+      <c r="I4" s="24">
         <f>AVERAGE(D36:D67)</f>
         <v>0.16034862587388751</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="B5" s="8"/>
       <c r="C5" s="8">
         <v>4</v>
@@ -1076,19 +1466,19 @@
         <v>5.1400000000000001E-2</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="7">
+      <c r="H5" s="7">
         <f>STDEV(D2:D35)</f>
         <v>0.21132785517347263</v>
       </c>
-      <c r="J5" s="7">
+      <c r="I5" s="7">
         <f>STDEV(D36:D67)</f>
         <v>0.32575035419397358</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="B6" s="8"/>
       <c r="C6" s="8">
         <v>5</v>
@@ -1098,7 +1488,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="B7" s="8"/>
       <c r="C7" s="8">
         <v>6</v>
@@ -1107,17 +1497,17 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="E7" s="2"/>
+      <c r="G7" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="H7" s="7" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="B8" s="8"/>
       <c r="C8" s="8">
         <v>7</v>
@@ -1126,19 +1516,19 @@
         <v>3.5740000000000001E-2</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="7">
+      <c r="H8" s="7">
         <f>COUNT(E2:E35)</f>
         <v>21</v>
       </c>
-      <c r="J8" s="7">
+      <c r="I8" s="7">
         <f>COUNT(E36:E67)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="B9" s="8"/>
       <c r="C9" s="8">
         <v>8</v>
@@ -1147,19 +1537,19 @@
         <v>2.1329999999999998E-2</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="H9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="7">
+      <c r="H9" s="7">
         <f>AVERAGE(E2:E35)</f>
         <v>0.10110664595549053</v>
       </c>
-      <c r="J9" s="24">
+      <c r="I9" s="24">
         <f>AVERAGE(E36:E67)</f>
         <v>4.9930767004645993E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="B10" s="8"/>
       <c r="C10" s="8">
         <v>9</v>
@@ -1168,19 +1558,19 @@
         <v>4.4863857697911916E-2</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="7">
+      <c r="H10" s="7">
         <f>STDEV(E2:E35)</f>
         <v>0.12270567866533642</v>
       </c>
-      <c r="J10" s="7">
+      <c r="I10" s="7">
         <f>STDEV(E36:E67)</f>
         <v>0.1098898005251446</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13">
       <c r="B11" s="8"/>
       <c r="C11" s="8">
         <v>10</v>
@@ -1190,7 +1580,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1">
       <c r="B12" s="8"/>
       <c r="C12" s="8">
         <v>11</v>
@@ -1199,14 +1589,14 @@
         <v>5.07077119821739E-2</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>42</v>
       </c>
-      <c r="L12" t="s">
+      <c r="K12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13">
       <c r="B13" s="8"/>
       <c r="C13" s="8">
         <v>12</v>
@@ -1215,22 +1605,22 @@
         <v>7.6398745049243919E-2</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37" t="s">
+      <c r="G13" s="36"/>
+      <c r="H13" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="I13" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="32"/>
-      <c r="M13" s="43" t="s">
+      <c r="K13" s="32"/>
+      <c r="L13" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="44" t="s">
+      <c r="M13" s="44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:13">
       <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
@@ -1246,26 +1636,26 @@
       <c r="E14" s="1">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="G14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="29">
+      <c r="H14" s="29">
         <v>0.17275404085692847</v>
       </c>
-      <c r="J14" s="30">
+      <c r="I14" s="30">
         <v>0.16034862587388751</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="K14" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="25">
+      <c r="L14" s="25">
         <v>0.10110664595549053</v>
       </c>
-      <c r="N14" s="34">
+      <c r="M14" s="34">
         <v>4.9930767004645993E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13">
       <c r="B15" s="8"/>
       <c r="C15" s="21" t="s">
         <v>17</v>
@@ -1276,26 +1666,26 @@
       <c r="E15" s="2">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="G15" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="29">
+      <c r="H15" s="29">
         <v>4.4659462372220224E-2</v>
       </c>
-      <c r="J15" s="30">
+      <c r="I15" s="30">
         <v>0.10611329325749923</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="K15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="25">
+      <c r="L15" s="25">
         <v>1.5056683576720797E-2</v>
       </c>
-      <c r="N15" s="34">
+      <c r="M15" s="34">
         <v>1.2075768259456072E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="B16" s="8"/>
       <c r="C16" s="21" t="s">
         <v>18</v>
@@ -1304,26 +1694,26 @@
       <c r="E16" s="2">
         <v>2.9100000000000001E-2</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="G16" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="29">
+      <c r="H16" s="29">
         <v>33</v>
       </c>
-      <c r="J16" s="30">
+      <c r="I16" s="30">
         <v>32</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="K16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="25">
+      <c r="L16" s="25">
         <v>21</v>
       </c>
-      <c r="N16" s="34">
+      <c r="M16" s="34">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:16">
       <c r="B17" s="8"/>
       <c r="C17" s="21" t="s">
         <v>19</v>
@@ -1332,24 +1722,24 @@
         <v>5.1691686177294215E-2</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="H17" s="28" t="s">
+      <c r="G17" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="29">
+      <c r="H17" s="29">
         <v>63</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="L17" s="33" t="s">
+      <c r="I17" s="30"/>
+      <c r="K17" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M17" s="25">
+      <c r="L17" s="25">
         <v>43</v>
       </c>
-      <c r="N17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="O17" s="47"/>
       <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-    </row>
-    <row r="18" spans="1:17">
+    </row>
+    <row r="18" spans="1:16">
       <c r="B18" s="8"/>
       <c r="C18" s="21" t="s">
         <v>20</v>
@@ -1360,24 +1750,24 @@
       <c r="E18" s="15">
         <v>2.4490821175140766E-2</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="G18" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="40">
+      <c r="H18" s="40">
         <v>0.1827046436141801</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="L18" s="41" t="s">
+      <c r="I18" s="30"/>
+      <c r="K18" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="42">
+      <c r="L18" s="42">
         <v>1.4760995551427978</v>
       </c>
-      <c r="N18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="O18" s="25"/>
       <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-    </row>
-    <row r="19" spans="1:17">
+    </row>
+    <row r="19" spans="1:16">
       <c r="B19" s="8"/>
       <c r="C19" s="21" t="s">
         <v>21</v>
@@ -1388,24 +1778,24 @@
       <c r="E19" s="15">
         <v>1.5903518653502084E-2</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="G19" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="40">
+      <c r="H19" s="40">
         <v>1.9983405224495088</v>
       </c>
-      <c r="J19" s="30"/>
-      <c r="L19" s="41" t="s">
+      <c r="I19" s="30"/>
+      <c r="K19" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="42">
+      <c r="L19" s="42">
         <v>2.0166921734373453</v>
       </c>
-      <c r="N19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="O19" s="47"/>
       <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-    </row>
-    <row r="20" spans="1:17">
+    </row>
+    <row r="20" spans="1:16">
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
         <v>13</v>
@@ -1414,24 +1804,24 @@
         <v>3.9086062452399081E-2</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="H20" s="39" t="s">
+      <c r="G20" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="40">
+      <c r="H20" s="40">
         <v>0.85561645176739187</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="L20" s="41" t="s">
+      <c r="I20" s="30"/>
+      <c r="K20" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="42">
+      <c r="L20" s="42">
         <v>0.14720323947750413</v>
       </c>
-      <c r="N20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="O20" s="25"/>
       <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1">
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1">
       <c r="B21" s="8"/>
       <c r="C21" s="21" t="s">
         <v>15</v>
@@ -1440,24 +1830,24 @@
         <v>8.6037735849056593E-2</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="H21" s="45" t="s">
+      <c r="G21" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="48">
-        <f>ROUND((1-I20),4)</f>
+      <c r="H21" s="48">
+        <f>ROUND((1-H20),4)</f>
         <v>0.1444</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="L21" s="46" t="s">
+      <c r="I21" s="31"/>
+      <c r="K21" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="M21" s="49">
-        <f>ROUND((1-M20),4)</f>
+      <c r="L21" s="49">
+        <f>ROUND((1-L20),4)</f>
         <v>0.8528</v>
       </c>
-      <c r="N21" s="35"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="M21" s="35"/>
+    </row>
+    <row r="22" spans="1:16">
       <c r="B22" s="8"/>
       <c r="C22" s="22" t="s">
         <v>14</v>
@@ -1467,7 +1857,7 @@
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1484,7 +1874,7 @@
         <v>0.19458874458874459</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:16">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8">
@@ -1497,7 +1887,7 @@
         <v>0.23342696629213483</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:16">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8">
@@ -1510,7 +1900,7 @@
         <v>8.6503067484662577E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:16">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8">
@@ -1523,7 +1913,7 @@
         <v>1.1335078534031413E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:16">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8">
@@ -1536,7 +1926,7 @@
         <v>1.7268518518518516E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:16">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8">
@@ -1549,7 +1939,7 @@
         <v>2.1363636363636362E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:16">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8">
@@ -1562,7 +1952,7 @@
         <v>1.3148148148148147E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:16">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8">
@@ -1575,7 +1965,7 @@
         <v>2.5677083333333333E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:16">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8">
@@ -1588,7 +1978,7 @@
         <v>3.7158469945355189E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:16">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8">
@@ -2046,6 +2436,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>